<commit_message>
added 2 new xlsx files
</commit_message>
<xml_diff>
--- a/api/scripts/files/round_1-A.xlsx
+++ b/api/scripts/files/round_1-A.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="764" uniqueCount="345">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="764" uniqueCount="350">
   <si>
     <t>sNo</t>
   </si>
@@ -40,7 +40,7 @@
     <t>filename</t>
   </si>
   <si>
-    <t>Identify the variant from which tilt steering is available in the vehicle shown above.</t>
+    <t>Identify the variant from which tilt steering is available in the vehicle shown here</t>
   </si>
   <si>
     <t>LXi</t>
@@ -79,7 +79,7 @@
     <t>2.mp4</t>
   </si>
   <si>
-    <t>What is the maximum power output of the vehicle shown above in Petrol? (kW @rpm)</t>
+    <t>What is the maximum power output of the vehicle shown here in Petrol? (kW @rpm)</t>
   </si>
   <si>
     <t>83 @ 6000</t>
@@ -97,7 +97,7 @@
     <t>3.jpg</t>
   </si>
   <si>
-    <t>The technology shown above is in which of following vehicles.</t>
+    <t>The technology shown here is in which of following vehicles.</t>
   </si>
   <si>
     <t>Alto K10</t>
@@ -115,7 +115,7 @@
     <t>4.png</t>
   </si>
   <si>
-    <t>What is the truning radius of the vehicle shown above in meters?</t>
+    <t>What is the turning radius of the vehicle shown here in meters?</t>
   </si>
   <si>
     <t>4.5 m</t>
@@ -133,7 +133,7 @@
     <t>5.jpg</t>
   </si>
   <si>
-    <t>Identify the variant from which the feature shown above is available.</t>
+    <t>Identify the variant from which the feature shown here is available.</t>
   </si>
   <si>
     <t>ZXi+</t>
@@ -157,7 +157,7 @@
     <t>7.mp4</t>
   </si>
   <si>
-    <t>What is the maximum torque output of the vehicle shown above in Petrol? (Nm@RPM)</t>
+    <t>What is the maximum torque output of the vehicle shown here in Petrol? (Nm@RPM)</t>
   </si>
   <si>
     <t>134.8 @ 4400</t>
@@ -175,7 +175,7 @@
     <t>8.png</t>
   </si>
   <si>
-    <t>Name this feature of Wagon R.</t>
+    <t>Name this feature of WagonR.</t>
   </si>
   <si>
     <t>Sporty Roof</t>
@@ -199,6 +199,9 @@
     <t>10.jpg</t>
   </si>
   <si>
+    <t>Identify the variant from which the feature shown in the image is available.</t>
+  </si>
+  <si>
     <t>11.jpg</t>
   </si>
   <si>
@@ -244,13 +247,13 @@
     <t>14.jpg</t>
   </si>
   <si>
-    <t>This feature comes from which variant in the vehicle shown above?</t>
+    <t>This feature comes from which variant in the vehicle shown here?</t>
   </si>
   <si>
     <t>15.jpg</t>
   </si>
   <si>
-    <t>Identify the variant from which the feature shown above is available in Alto</t>
+    <t>Identify the variant from which the feature shown in the image is available in Alto</t>
   </si>
   <si>
     <t>VXi+</t>
@@ -298,13 +301,13 @@
     <t>19.jpg</t>
   </si>
   <si>
-    <t>What is the length of the vehicle shown above? (mm)</t>
+    <t>What is the length of the vehicle shown in the image? (mm)</t>
   </si>
   <si>
     <t>20.jpg</t>
   </si>
   <si>
-    <t>Identify the variant of Brezza in which the wheels shown above are available?</t>
+    <t>Identify the variant of Brezza in which the wheels shown in the image are available.</t>
   </si>
   <si>
     <t>21.png</t>
@@ -328,7 +331,7 @@
     <t>22.mp4</t>
   </si>
   <si>
-    <t>From which variant of Brezza is the feature shown above available</t>
+    <t>From which variant of Brezza is the feature shown in the image available</t>
   </si>
   <si>
     <t>ZXI+</t>
@@ -337,13 +340,13 @@
     <t>23.jpg</t>
   </si>
   <si>
-    <t>What is the turning radius of the vehicle shown above in Petrol? (m)</t>
+    <t>What is the turning radius of the vehicle shown in the image in Petrol? (m)</t>
   </si>
   <si>
     <t>24.png</t>
   </si>
   <si>
-    <t>What is the mileage of the vehicle shown above in Petrol? (kmpl)</t>
+    <t>What is the mileage of the vehicle shown in the image in Petrol? (kmpl)</t>
   </si>
   <si>
     <t>25.png</t>
@@ -379,7 +382,7 @@
     <t>28.png</t>
   </si>
   <si>
-    <t>This feature shown above is in which of following vehicles.</t>
+    <t>This feature shown here is in which of the following vehicles?</t>
   </si>
   <si>
     <t>29.png</t>
@@ -388,7 +391,7 @@
     <t>What is the size of the wheel shown in the image.</t>
   </si>
   <si>
-    <t>30.png</t>
+    <t>30.jpg</t>
   </si>
   <si>
     <t>31.jpg</t>
@@ -409,7 +412,7 @@
     <t>32.mp4</t>
   </si>
   <si>
-    <t>What is the engine capacity of the vehicle shown above? (cc)</t>
+    <t>What is the engine capacity of the vehicle shown here? (cc)</t>
   </si>
   <si>
     <t>33.png</t>
@@ -427,13 +430,13 @@
     <t>34.mp4</t>
   </si>
   <si>
-    <t>What is the turning radius ofof the vehicle shown above? (m)</t>
+    <t>What is the turning radius ofof the vehicle shown in the image? (m)</t>
   </si>
   <si>
     <t>35.png</t>
   </si>
   <si>
-    <t>In which variant is the feature shown above available in S-Presso.</t>
+    <t>In which variant is the feature shown in the image available in S-Presso?</t>
   </si>
   <si>
     <t>36.png</t>
@@ -454,16 +457,19 @@
     <t>37.mp4</t>
   </si>
   <si>
-    <t>What is the boot space of of the vehicle shown above? (L)</t>
+    <t>What is the boot space of the vehicle shown here? (L)</t>
   </si>
   <si>
     <t>38.jpg</t>
   </si>
   <si>
+    <t>This feature shown here is in which of the following vehicles.</t>
+  </si>
+  <si>
     <t>39.jpg</t>
   </si>
   <si>
-    <t>What is the Mileage of the vehicle shown above in Petrol (Lxi, MT)? (kmpl)</t>
+    <t>What is the Mileage of the vehicle shown in the image in Petrol (Lxi, MT)? (kmpl)</t>
   </si>
   <si>
     <t>40.png</t>
@@ -487,7 +493,7 @@
     <t>42.mp4</t>
   </si>
   <si>
-    <t>What is the maximum power output of the vehicle shown above in CNG? (kW@rpm)</t>
+    <t>What is the maximum power output of the vehicle shown image in CNG? (kW@rpm)</t>
   </si>
   <si>
     <t>43.2 @ 5300</t>
@@ -508,7 +514,7 @@
     <t>44.jpg</t>
   </si>
   <si>
-    <t>What is the Mileage of the vehicle shown above in CNG? (km/kg)</t>
+    <t>What is the Mileage of the vehicle shown here in CNG? (km/kg)</t>
   </si>
   <si>
     <t>45.jpg</t>
@@ -532,7 +538,7 @@
     <t>47.mp4</t>
   </si>
   <si>
-    <t>What is the Mileage of the vehicle shown above in Petrol? (kmpl)</t>
+    <t>What is the Mileage of the vehicle shown in the image in Petrol? (kmpl)</t>
   </si>
   <si>
     <t>24.39 MT</t>
@@ -556,7 +562,7 @@
     <t>49.jpg</t>
   </si>
   <si>
-    <t>What is the name of the feature shownn above in Dzire?</t>
+    <t>What is the name of the feature shown here in Dzire?</t>
   </si>
   <si>
     <t>Premium single aperture Grille</t>
@@ -574,7 +580,7 @@
     <t>50.png</t>
   </si>
   <si>
-    <t>Identify the variant from which the feature shown above is available in Ertiga</t>
+    <t>Identify the variant from which the feature shown in the image is available in Ertiga.</t>
   </si>
   <si>
     <t>51.png</t>
@@ -592,25 +598,25 @@
     <t>52.mp4</t>
   </si>
   <si>
-    <t>What is the boot capacity of the vehicle shown above? (L)</t>
+    <t>What is the boot capacity of the vehicle shown here? (L)</t>
   </si>
   <si>
     <t>53.png</t>
   </si>
   <si>
-    <t>The feature/technology shown above is available in which of the following vehicles.</t>
+    <t>The feature/technology shown here is available in which of the following vehicles?</t>
   </si>
   <si>
     <t>54.jpg</t>
   </si>
   <si>
-    <t>What is the turning radius of the vehicle shown above? (m)</t>
+    <t>What is the turning radius of the vehicle shown here? (m)</t>
   </si>
   <si>
     <t>55.jpg</t>
   </si>
   <si>
-    <t>Identify the variant from which the feature shown above is available in Dzire</t>
+    <t>Identify the variant from which the feature shown in the image is available in Dzire</t>
   </si>
   <si>
     <t>56.jpg</t>
@@ -631,19 +637,22 @@
     <t>57.mp4</t>
   </si>
   <si>
+    <t>What is the Mileage of the vehicle shown in the image in CNG? (km/kg)</t>
+  </si>
+  <si>
     <t>58.jpg</t>
   </si>
   <si>
     <t>59.png</t>
   </si>
   <si>
-    <t>What is the Mileage of the vehicle shown above in Petrol, AGS? (kmpl)</t>
+    <t>What is the Mileage of the vehicle shown in the image in Petrol, AGS? (kmpl)</t>
   </si>
   <si>
     <t>60.jpg</t>
   </si>
   <si>
-    <t>In which variant is the feature shown above available in Swift.</t>
+    <t>In which variant is the feature shown here available in Swift?</t>
   </si>
   <si>
     <t>61.jpg</t>
@@ -676,7 +685,7 @@
     <t>65.png</t>
   </si>
   <si>
-    <t>From which variant of Brezza is the feature shown above available.</t>
+    <t>From which variant of Brezza is the feature shown in the image available.</t>
   </si>
   <si>
     <t>All of the above</t>
@@ -685,7 +694,7 @@
     <t>66.jpg</t>
   </si>
   <si>
-    <t>Which of thesefeatures adds to comfort on highways?</t>
+    <t>Which of these features adds to comfort on highways?</t>
   </si>
   <si>
     <t>Remote keyless entry</t>
@@ -700,6 +709,9 @@
     <t>67.mp4</t>
   </si>
   <si>
+    <t>What is the maximum power output of the vehicle shown in the image in CNG? (kW@rpm)</t>
+  </si>
+  <si>
     <t>120.5 @ 4500</t>
   </si>
   <si>
@@ -715,7 +727,7 @@
     <t>68.png</t>
   </si>
   <si>
-    <t>What is the application shown above?</t>
+    <t>What is the application shown in the image?</t>
   </si>
   <si>
     <t>Media</t>
@@ -733,13 +745,13 @@
     <t>69.png</t>
   </si>
   <si>
-    <t>What is the Mileage of the vehicle shown above in 1.0 L, AGS Petrol? (kmpl)</t>
+    <t>What is the Mileage of the vehicle shown in the image in 1.0 L, AGS Petrol? (kmpl)</t>
   </si>
   <si>
     <t>70.png</t>
   </si>
   <si>
-    <t>From which variant is rear parcel tray available in the vehicle shown aboveo?</t>
+    <t>From which variant is the rear parcel tray available in the vehicle shown in the image?</t>
   </si>
   <si>
     <t>71.png</t>
@@ -754,7 +766,7 @@
     <t>72.mp4</t>
   </si>
   <si>
-    <t>What is the torque output of the vehicle shown above in CNG? (Nm@RPM)</t>
+    <t>What is the torque output of the vehicle shown in the image in CNG? (Nm@RPM)</t>
   </si>
   <si>
     <t>84.1 @ 3500</t>
@@ -772,16 +784,16 @@
     <t>73.jpg</t>
   </si>
   <si>
-    <t>This technology/feature shown above is in which of following vehicles.</t>
+    <t>This technology/feature shown in the image is in which of the following vehicles?</t>
   </si>
   <si>
     <t>74.jpg</t>
   </si>
   <si>
-    <t>75.tif</t>
-  </si>
-  <si>
-    <t>From which variant are front fog lamps available in the vehicle shown above?</t>
+    <t>75.png</t>
+  </si>
+  <si>
+    <t>From which variant are front fog lamps available in the vehicle shown here?</t>
   </si>
   <si>
     <t>76.png</t>
@@ -823,7 +835,7 @@
     <t>80.jpg</t>
   </si>
   <si>
-    <t>Identify the stroke shown in the snippet.</t>
+    <t>Identify the stroke shown in the image.</t>
   </si>
   <si>
     <t>Intake</t>
@@ -850,36 +862,39 @@
     <t>84.png</t>
   </si>
   <si>
+    <t>This engine has __ valves.</t>
+  </si>
+  <si>
+    <t>85.png</t>
+  </si>
+  <si>
+    <t>86.png</t>
+  </si>
+  <si>
+    <t>In which vehicle will you find the technology shown?</t>
+  </si>
+  <si>
+    <t>87.mp4</t>
+  </si>
+  <si>
+    <t>The engine of this vehicle is also available in______.</t>
+  </si>
+  <si>
+    <t>88.mp4</t>
+  </si>
+  <si>
+    <t>89.mp4</t>
+  </si>
+  <si>
+    <t>Alto K-10</t>
+  </si>
+  <si>
+    <t>90.mp4</t>
+  </si>
+  <si>
     <t>The engine of this vehicle has __ valves.</t>
   </si>
   <si>
-    <t>85.png</t>
-  </si>
-  <si>
-    <t>86.png</t>
-  </si>
-  <si>
-    <t>In which vehicle will you find the technology shown?</t>
-  </si>
-  <si>
-    <t>87.mp4</t>
-  </si>
-  <si>
-    <t>The engine of this vehicle is also available in______.</t>
-  </si>
-  <si>
-    <t>88.mp4</t>
-  </si>
-  <si>
-    <t>89.mp4</t>
-  </si>
-  <si>
-    <t>Alto K-10</t>
-  </si>
-  <si>
-    <t>90.mp4</t>
-  </si>
-  <si>
     <t>91.mp4</t>
   </si>
   <si>
@@ -895,7 +910,7 @@
     <t>93.mp4</t>
   </si>
   <si>
-    <t>Identify the feature/ technology shown in the snippet.</t>
+    <t>Identify the feature/ technology shown in the image.</t>
   </si>
   <si>
     <t>EBD</t>
@@ -904,7 +919,7 @@
     <t>94.png</t>
   </si>
   <si>
-    <t>Identify the feature/ technology of shown in the snippet.</t>
+    <t>Identify the feature/ technology of shown in the image.</t>
   </si>
   <si>
     <t>95.png</t>
@@ -1052,7 +1067,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -1065,6 +1080,12 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11.0"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11.0"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -1128,7 +1149,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -1164,6 +1185,9 @@
     </xf>
     <xf borderId="4" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="right" readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="4" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1708,7 +1732,7 @@
         <v>11.0</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>40</v>
+        <v>62</v>
       </c>
       <c r="C12" s="8" t="s">
         <v>10</v>
@@ -1729,7 +1753,7 @@
         <v>13</v>
       </c>
       <c r="I12" s="9" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="13">
@@ -1737,16 +1761,16 @@
         <v>12.0</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D13" s="9" t="s">
         <v>43</v>
       </c>
       <c r="E13" s="9" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="F13" s="9" t="s">
         <v>17</v>
@@ -1758,7 +1782,7 @@
         <v>20</v>
       </c>
       <c r="I13" s="9" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="14">
@@ -1769,25 +1793,25 @@
         <v>48</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D14" s="9" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="E14" s="9" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="F14" s="9" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="G14" s="9" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="H14" s="9" t="s">
         <v>13</v>
       </c>
       <c r="I14" s="9" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="15">
@@ -1795,19 +1819,19 @@
         <v>14.0</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D15" s="9" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="E15" s="9" t="s">
         <v>31</v>
       </c>
       <c r="F15" s="9" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="G15" s="9" t="s">
         <v>31</v>
@@ -1816,7 +1840,7 @@
         <v>13</v>
       </c>
       <c r="I15" s="9" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="16">
@@ -1824,7 +1848,7 @@
         <v>15.0</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C16" s="8" t="s">
         <v>11</v>
@@ -1845,7 +1869,7 @@
         <v>13</v>
       </c>
       <c r="I16" s="9" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="17">
@@ -1853,7 +1877,7 @@
         <v>16.0</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C17" s="8" t="s">
         <v>10</v>
@@ -1862,19 +1886,19 @@
         <v>11</v>
       </c>
       <c r="E17" s="9" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="F17" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="G17" s="9" t="s">
         <v>81</v>
       </c>
-      <c r="G17" s="9" t="s">
-        <v>80</v>
-      </c>
       <c r="H17" s="9" t="s">
         <v>13</v>
       </c>
       <c r="I17" s="9" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="18">
@@ -1882,28 +1906,28 @@
         <v>17.0</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C18" s="8" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D18" s="9" t="s">
         <v>17</v>
       </c>
       <c r="E18" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="F18" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="G18" s="9" t="s">
         <v>84</v>
-      </c>
-      <c r="F18" s="9" t="s">
-        <v>85</v>
-      </c>
-      <c r="G18" s="9" t="s">
-        <v>83</v>
       </c>
       <c r="H18" s="9" t="s">
         <v>20</v>
       </c>
       <c r="I18" s="9" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row r="19">
@@ -1911,28 +1935,28 @@
         <v>18.0</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C19" s="8" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D19" s="9" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="E19" s="9" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="F19" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="G19" s="9" t="s">
         <v>90</v>
       </c>
-      <c r="G19" s="9" t="s">
-        <v>89</v>
-      </c>
       <c r="H19" s="9" t="s">
         <v>13</v>
       </c>
       <c r="I19" s="9" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
     </row>
     <row r="20">
@@ -1940,16 +1964,16 @@
         <v>19.0</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C20" s="8" t="s">
         <v>31</v>
       </c>
       <c r="D20" s="9" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="E20" s="9" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="F20" s="9" t="s">
         <v>32</v>
@@ -1961,7 +1985,7 @@
         <v>13</v>
       </c>
       <c r="I20" s="9" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
     <row r="21">
@@ -1969,7 +1993,7 @@
         <v>20.0</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C21" s="10">
         <v>3565.0</v>
@@ -1990,7 +2014,7 @@
         <v>13</v>
       </c>
       <c r="I21" s="9" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
     </row>
     <row r="22">
@@ -1998,7 +2022,7 @@
         <v>21.0</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C22" s="8" t="s">
         <v>10</v>
@@ -2019,7 +2043,7 @@
         <v>13</v>
       </c>
       <c r="I22" s="9" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row r="23">
@@ -2027,28 +2051,28 @@
         <v>22.0</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C23" s="8" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="D23" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="E23" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="F23" s="9" t="s">
+        <v>104</v>
+      </c>
+      <c r="G23" s="9" t="s">
         <v>101</v>
-      </c>
-      <c r="E23" s="9" t="s">
-        <v>102</v>
-      </c>
-      <c r="F23" s="9" t="s">
-        <v>103</v>
-      </c>
-      <c r="G23" s="9" t="s">
-        <v>100</v>
       </c>
       <c r="H23" s="9" t="s">
         <v>20</v>
       </c>
       <c r="I23" s="9" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
     </row>
     <row r="24">
@@ -2056,28 +2080,28 @@
         <v>23.0</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="C24" s="8" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D24" s="9" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="E24" s="9" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="F24" s="9" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="G24" s="9" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="H24" s="9" t="s">
         <v>13</v>
       </c>
       <c r="I24" s="9" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
     </row>
     <row r="25">
@@ -2085,7 +2109,7 @@
         <v>24.0</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="C25" s="10">
         <v>4.8</v>
@@ -2106,7 +2130,7 @@
         <v>13</v>
       </c>
       <c r="I25" s="9" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
     </row>
     <row r="26">
@@ -2114,7 +2138,7 @@
         <v>25.0</v>
       </c>
       <c r="B26" s="7" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="C26" s="10">
         <v>18.71</v>
@@ -2135,7 +2159,7 @@
         <v>13</v>
       </c>
       <c r="I26" s="9" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
     </row>
     <row r="27">
@@ -2143,7 +2167,7 @@
         <v>26.0</v>
       </c>
       <c r="B27" s="7" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="C27" s="8" t="s">
         <v>10</v>
@@ -2164,7 +2188,7 @@
         <v>13</v>
       </c>
       <c r="I27" s="9" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
     <row r="28">
@@ -2172,28 +2196,28 @@
         <v>27.0</v>
       </c>
       <c r="B28" s="7" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="C28" s="8" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="D28" s="9" t="s">
+        <v>117</v>
+      </c>
+      <c r="E28" s="9" t="s">
+        <v>118</v>
+      </c>
+      <c r="F28" s="9" t="s">
+        <v>119</v>
+      </c>
+      <c r="G28" s="9" t="s">
         <v>116</v>
-      </c>
-      <c r="E28" s="9" t="s">
-        <v>117</v>
-      </c>
-      <c r="F28" s="9" t="s">
-        <v>118</v>
-      </c>
-      <c r="G28" s="9" t="s">
-        <v>115</v>
       </c>
       <c r="H28" s="9" t="s">
         <v>20</v>
       </c>
       <c r="I28" s="9" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
     </row>
     <row r="29">
@@ -2201,7 +2225,7 @@
         <v>28.0</v>
       </c>
       <c r="B29" s="7" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="C29" s="10">
         <v>998.0</v>
@@ -2222,7 +2246,7 @@
         <v>13</v>
       </c>
       <c r="I29" s="9" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
     </row>
     <row r="30">
@@ -2230,28 +2254,28 @@
         <v>29.0</v>
       </c>
       <c r="B30" s="7" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="C30" s="8" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D30" s="9" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="E30" s="9" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="F30" s="9" t="s">
         <v>29</v>
       </c>
       <c r="G30" s="9" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="H30" s="9" t="s">
         <v>13</v>
       </c>
       <c r="I30" s="9" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
     </row>
     <row r="31">
@@ -2259,7 +2283,7 @@
         <v>30.0</v>
       </c>
       <c r="B31" s="7" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C31" s="10">
         <v>15.0</v>
@@ -2280,7 +2304,7 @@
         <v>13</v>
       </c>
       <c r="I31" s="9" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
     </row>
     <row r="32">
@@ -2288,7 +2312,7 @@
         <v>31.0</v>
       </c>
       <c r="B32" s="7" t="s">
-        <v>40</v>
+        <v>62</v>
       </c>
       <c r="C32" s="8" t="s">
         <v>10</v>
@@ -2309,7 +2333,7 @@
         <v>13</v>
       </c>
       <c r="I32" s="9" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
     </row>
     <row r="33">
@@ -2317,28 +2341,28 @@
         <v>32.0</v>
       </c>
       <c r="B33" s="7" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C33" s="8" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="D33" s="9" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="E33" s="9" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="F33" s="9" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="G33" s="9" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="H33" s="9" t="s">
         <v>20</v>
       </c>
       <c r="I33" s="9" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
     </row>
     <row r="34">
@@ -2346,7 +2370,7 @@
         <v>33.0</v>
       </c>
       <c r="B34" s="7" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="C34" s="10">
         <v>1100.0</v>
@@ -2367,7 +2391,7 @@
         <v>13</v>
       </c>
       <c r="I34" s="9" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
     </row>
     <row r="35">
@@ -2375,19 +2399,19 @@
         <v>34.0</v>
       </c>
       <c r="B35" s="7" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="C35" s="8" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D35" s="9" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="E35" s="9" t="s">
         <v>30</v>
       </c>
       <c r="F35" s="9" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="G35" s="9" t="s">
         <v>30</v>
@@ -2396,7 +2420,7 @@
         <v>20</v>
       </c>
       <c r="I35" s="9" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
     </row>
     <row r="36">
@@ -2404,7 +2428,7 @@
         <v>35.0</v>
       </c>
       <c r="B36" s="7" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="C36" s="10">
         <v>5.1</v>
@@ -2425,7 +2449,7 @@
         <v>13</v>
       </c>
       <c r="I36" s="9" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
     </row>
     <row r="37">
@@ -2433,7 +2457,7 @@
         <v>36.0</v>
       </c>
       <c r="B37" s="7" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="C37" s="8" t="s">
         <v>10</v>
@@ -2442,10 +2466,10 @@
         <v>11</v>
       </c>
       <c r="E37" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="F37" s="9" t="s">
         <v>81</v>
-      </c>
-      <c r="F37" s="9" t="s">
-        <v>80</v>
       </c>
       <c r="G37" s="9" t="s">
         <v>11</v>
@@ -2454,7 +2478,7 @@
         <v>13</v>
       </c>
       <c r="I37" s="9" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
     </row>
     <row r="38">
@@ -2462,28 +2486,28 @@
         <v>37.0</v>
       </c>
       <c r="B38" s="7" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C38" s="8" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="D38" s="9" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="E38" s="9" t="s">
+        <v>145</v>
+      </c>
+      <c r="F38" s="9" t="s">
+        <v>146</v>
+      </c>
+      <c r="G38" s="9" t="s">
         <v>144</v>
-      </c>
-      <c r="F38" s="9" t="s">
-        <v>145</v>
-      </c>
-      <c r="G38" s="9" t="s">
-        <v>143</v>
       </c>
       <c r="H38" s="9" t="s">
         <v>20</v>
       </c>
       <c r="I38" s="9" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
     </row>
     <row r="39">
@@ -2491,7 +2515,7 @@
         <v>38.0</v>
       </c>
       <c r="B39" s="7" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="C39" s="10">
         <v>260.0</v>
@@ -2512,7 +2536,7 @@
         <v>13</v>
       </c>
       <c r="I39" s="9" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
     </row>
     <row r="40">
@@ -2520,28 +2544,28 @@
         <v>39.0</v>
       </c>
       <c r="B40" s="7" t="s">
-        <v>122</v>
+        <v>150</v>
       </c>
       <c r="C40" s="8" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D40" s="9" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="E40" s="9" t="s">
         <v>29</v>
       </c>
       <c r="F40" s="9" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="G40" s="9" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="H40" s="9" t="s">
         <v>13</v>
       </c>
       <c r="I40" s="9" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
     </row>
     <row r="41">
@@ -2549,7 +2573,7 @@
         <v>40.0</v>
       </c>
       <c r="B41" s="7" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="C41" s="10">
         <v>18.51</v>
@@ -2570,7 +2594,7 @@
         <v>13</v>
       </c>
       <c r="I41" s="9" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
     </row>
     <row r="42">
@@ -2578,7 +2602,7 @@
         <v>41.0</v>
       </c>
       <c r="B42" s="7" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="C42" s="8" t="s">
         <v>10</v>
@@ -2599,7 +2623,7 @@
         <v>13</v>
       </c>
       <c r="I42" s="9" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
     </row>
     <row r="43">
@@ -2607,28 +2631,28 @@
         <v>42.0</v>
       </c>
       <c r="B43" s="7" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="C43" s="8" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="D43" s="9" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="E43" s="9" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="F43" s="9" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="G43" s="9" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="H43" s="9" t="s">
         <v>20</v>
       </c>
       <c r="I43" s="9" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
     </row>
     <row r="44">
@@ -2636,28 +2660,28 @@
         <v>43.0</v>
       </c>
       <c r="B44" s="7" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="C44" s="8" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="D44" s="9" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="E44" s="9" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="F44" s="9" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="G44" s="9" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="H44" s="9" t="s">
         <v>13</v>
       </c>
       <c r="I44" s="9" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
     </row>
     <row r="45">
@@ -2665,28 +2689,28 @@
         <v>44.0</v>
       </c>
       <c r="B45" s="7" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="C45" s="8" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D45" s="9" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="E45" s="9" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="F45" s="9" t="s">
         <v>31</v>
       </c>
       <c r="G45" s="9" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="H45" s="9" t="s">
         <v>13</v>
       </c>
       <c r="I45" s="9" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
     </row>
     <row r="46">
@@ -2694,7 +2718,7 @@
         <v>45.0</v>
       </c>
       <c r="B46" s="7" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="C46" s="10">
         <v>24.12</v>
@@ -2715,7 +2739,7 @@
         <v>13</v>
       </c>
       <c r="I46" s="9" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
     </row>
     <row r="47">
@@ -2723,7 +2747,7 @@
         <v>46.0</v>
       </c>
       <c r="B47" s="7" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="C47" s="10">
         <v>998.0</v>
@@ -2744,7 +2768,7 @@
         <v>13</v>
       </c>
       <c r="I47" s="9" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
     </row>
     <row r="48">
@@ -2752,28 +2776,28 @@
         <v>47.0</v>
       </c>
       <c r="B48" s="7" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="C48" s="8" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="D48" s="9" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="E48" s="9" t="s">
+        <v>172</v>
+      </c>
+      <c r="F48" s="9" t="s">
+        <v>173</v>
+      </c>
+      <c r="G48" s="9" t="s">
         <v>170</v>
-      </c>
-      <c r="F48" s="9" t="s">
-        <v>171</v>
-      </c>
-      <c r="G48" s="9" t="s">
-        <v>168</v>
       </c>
       <c r="H48" s="9" t="s">
         <v>20</v>
       </c>
       <c r="I48" s="9" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
     </row>
     <row r="49">
@@ -2781,28 +2805,28 @@
         <v>48.0</v>
       </c>
       <c r="B49" s="7" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="C49" s="8" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="D49" s="9" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="E49" s="9" t="s">
+        <v>178</v>
+      </c>
+      <c r="F49" s="9" t="s">
+        <v>179</v>
+      </c>
+      <c r="G49" s="9" t="s">
         <v>176</v>
       </c>
-      <c r="F49" s="9" t="s">
-        <v>177</v>
-      </c>
-      <c r="G49" s="9" t="s">
-        <v>174</v>
-      </c>
       <c r="H49" s="9" t="s">
         <v>13</v>
       </c>
       <c r="I49" s="9" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
     </row>
     <row r="50">
@@ -2810,16 +2834,16 @@
         <v>49.0</v>
       </c>
       <c r="B50" s="7" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="C50" s="8" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="D50" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="E50" s="9" t="s">
         <v>75</v>
-      </c>
-      <c r="E50" s="9" t="s">
-        <v>74</v>
       </c>
       <c r="F50" s="9" t="s">
         <v>30</v>
@@ -2831,7 +2855,7 @@
         <v>13</v>
       </c>
       <c r="I50" s="9" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
     </row>
     <row r="51">
@@ -2839,28 +2863,28 @@
         <v>50.0</v>
       </c>
       <c r="B51" s="7" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="C51" s="8" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="D51" s="9" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="E51" s="9" t="s">
+        <v>186</v>
+      </c>
+      <c r="F51" s="9" t="s">
+        <v>187</v>
+      </c>
+      <c r="G51" s="9" t="s">
         <v>184</v>
       </c>
-      <c r="F51" s="9" t="s">
-        <v>185</v>
-      </c>
-      <c r="G51" s="9" t="s">
-        <v>182</v>
-      </c>
       <c r="H51" s="9" t="s">
         <v>13</v>
       </c>
       <c r="I51" s="9" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
     </row>
     <row r="52">
@@ -2868,7 +2892,7 @@
         <v>51.0</v>
       </c>
       <c r="B52" s="7" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="C52" s="8" t="s">
         <v>10</v>
@@ -2889,7 +2913,7 @@
         <v>13</v>
       </c>
       <c r="I52" s="9" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
     </row>
     <row r="53">
@@ -2897,28 +2921,28 @@
         <v>52.0</v>
       </c>
       <c r="B53" s="7" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="C53" s="8" t="s">
         <v>19</v>
       </c>
       <c r="D53" s="9" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="E53" s="9" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="F53" s="9" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="G53" s="9" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="H53" s="9" t="s">
         <v>20</v>
       </c>
       <c r="I53" s="9" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
     </row>
     <row r="54">
@@ -2926,7 +2950,7 @@
         <v>53.0</v>
       </c>
       <c r="B54" s="7" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="C54" s="10">
         <v>384.0</v>
@@ -2947,7 +2971,7 @@
         <v>13</v>
       </c>
       <c r="I54" s="9" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
     </row>
     <row r="55">
@@ -2955,10 +2979,10 @@
         <v>54.0</v>
       </c>
       <c r="B55" s="7" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="C55" s="8" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D55" s="9" t="s">
         <v>30</v>
@@ -2967,7 +2991,7 @@
         <v>29</v>
       </c>
       <c r="F55" s="9" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="G55" s="9" t="s">
         <v>29</v>
@@ -2976,7 +3000,7 @@
         <v>13</v>
       </c>
       <c r="I55" s="9" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
     </row>
     <row r="56">
@@ -2984,7 +3008,7 @@
         <v>55.0</v>
       </c>
       <c r="B56" s="7" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="C56" s="10">
         <v>4.7</v>
@@ -3005,7 +3029,7 @@
         <v>13</v>
       </c>
       <c r="I56" s="9" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
     </row>
     <row r="57">
@@ -3013,7 +3037,7 @@
         <v>56.0</v>
       </c>
       <c r="B57" s="7" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="C57" s="8" t="s">
         <v>10</v>
@@ -3034,7 +3058,7 @@
         <v>13</v>
       </c>
       <c r="I57" s="9" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
     </row>
     <row r="58">
@@ -3042,28 +3066,28 @@
         <v>57.0</v>
       </c>
       <c r="B58" s="7" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="C58" s="8" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="D58" s="9" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="E58" s="9" t="s">
+        <v>205</v>
+      </c>
+      <c r="F58" s="9" t="s">
+        <v>206</v>
+      </c>
+      <c r="G58" s="9" t="s">
         <v>203</v>
-      </c>
-      <c r="F58" s="9" t="s">
-        <v>204</v>
-      </c>
-      <c r="G58" s="9" t="s">
-        <v>201</v>
       </c>
       <c r="H58" s="9" t="s">
         <v>20</v>
       </c>
       <c r="I58" s="9" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
     </row>
     <row r="59">
@@ -3071,7 +3095,7 @@
         <v>58.0</v>
       </c>
       <c r="B59" s="7" t="s">
-        <v>165</v>
+        <v>208</v>
       </c>
       <c r="C59" s="10">
         <v>30.1</v>
@@ -3092,7 +3116,7 @@
         <v>13</v>
       </c>
       <c r="I59" s="9" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
     </row>
     <row r="60">
@@ -3100,7 +3124,7 @@
         <v>59.0</v>
       </c>
       <c r="B60" s="7" t="s">
-        <v>165</v>
+        <v>208</v>
       </c>
       <c r="C60" s="10">
         <v>26.78</v>
@@ -3121,7 +3145,7 @@
         <v>13</v>
       </c>
       <c r="I60" s="9" t="s">
-        <v>207</v>
+        <v>210</v>
       </c>
     </row>
     <row r="61">
@@ -3129,7 +3153,7 @@
         <v>60.0</v>
       </c>
       <c r="B61" s="7" t="s">
-        <v>208</v>
+        <v>211</v>
       </c>
       <c r="C61" s="10">
         <v>24.12</v>
@@ -3150,7 +3174,7 @@
         <v>13</v>
       </c>
       <c r="I61" s="9" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
     </row>
     <row r="62">
@@ -3158,7 +3182,7 @@
         <v>61.0</v>
       </c>
       <c r="B62" s="7" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
       <c r="C62" s="8" t="s">
         <v>10</v>
@@ -3179,7 +3203,7 @@
         <v>13</v>
       </c>
       <c r="I62" s="9" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
     </row>
     <row r="63">
@@ -3187,28 +3211,28 @@
         <v>62.0</v>
       </c>
       <c r="B63" s="7" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C63" s="8" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="D63" s="9" t="s">
-        <v>213</v>
+        <v>216</v>
       </c>
       <c r="E63" s="9" t="s">
-        <v>214</v>
+        <v>217</v>
       </c>
       <c r="F63" s="9" t="s">
+        <v>218</v>
+      </c>
+      <c r="G63" s="9" t="s">
         <v>215</v>
-      </c>
-      <c r="G63" s="9" t="s">
-        <v>212</v>
       </c>
       <c r="H63" s="9" t="s">
         <v>20</v>
       </c>
       <c r="I63" s="9" t="s">
-        <v>216</v>
+        <v>219</v>
       </c>
     </row>
     <row r="64">
@@ -3216,7 +3240,7 @@
         <v>63.0</v>
       </c>
       <c r="B64" s="7" t="s">
-        <v>165</v>
+        <v>208</v>
       </c>
       <c r="C64" s="10">
         <v>30.6</v>
@@ -3237,7 +3261,7 @@
         <v>13</v>
       </c>
       <c r="I64" s="9" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
     </row>
     <row r="65">
@@ -3245,7 +3269,7 @@
         <v>64.0</v>
       </c>
       <c r="B65" s="7" t="s">
-        <v>218</v>
+        <v>221</v>
       </c>
       <c r="C65" s="10">
         <v>4.0</v>
@@ -3266,7 +3290,7 @@
         <v>13</v>
       </c>
       <c r="I65" s="9" t="s">
-        <v>219</v>
+        <v>222</v>
       </c>
     </row>
     <row r="66">
@@ -3274,7 +3298,7 @@
         <v>65.0</v>
       </c>
       <c r="B66" s="7" t="s">
-        <v>165</v>
+        <v>208</v>
       </c>
       <c r="C66" s="10">
         <v>30.05</v>
@@ -3295,7 +3319,7 @@
         <v>13</v>
       </c>
       <c r="I66" s="9" t="s">
-        <v>220</v>
+        <v>223</v>
       </c>
     </row>
     <row r="67">
@@ -3303,7 +3327,7 @@
         <v>66.0</v>
       </c>
       <c r="B67" s="7" t="s">
-        <v>221</v>
+        <v>224</v>
       </c>
       <c r="C67" s="8" t="s">
         <v>10</v>
@@ -3315,7 +3339,7 @@
         <v>12</v>
       </c>
       <c r="F67" s="9" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="G67" s="9" t="s">
         <v>12</v>
@@ -3324,7 +3348,7 @@
         <v>13</v>
       </c>
       <c r="I67" s="9" t="s">
-        <v>223</v>
+        <v>226</v>
       </c>
     </row>
     <row r="68">
@@ -3332,28 +3356,28 @@
         <v>67.0</v>
       </c>
       <c r="B68" s="7" t="s">
-        <v>224</v>
+        <v>227</v>
       </c>
       <c r="C68" s="8" t="s">
-        <v>225</v>
+        <v>228</v>
       </c>
       <c r="D68" s="9" t="s">
-        <v>226</v>
+        <v>229</v>
       </c>
       <c r="E68" s="9" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="F68" s="9" t="s">
-        <v>227</v>
+        <v>230</v>
       </c>
       <c r="G68" s="9" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="H68" s="9" t="s">
         <v>20</v>
       </c>
       <c r="I68" s="9" t="s">
-        <v>228</v>
+        <v>231</v>
       </c>
     </row>
     <row r="69">
@@ -3361,28 +3385,28 @@
         <v>68.0</v>
       </c>
       <c r="B69" s="7" t="s">
-        <v>158</v>
+        <v>232</v>
       </c>
       <c r="C69" s="8" t="s">
-        <v>229</v>
+        <v>233</v>
       </c>
       <c r="D69" s="9" t="s">
-        <v>230</v>
+        <v>234</v>
       </c>
       <c r="E69" s="9" t="s">
-        <v>231</v>
+        <v>235</v>
       </c>
       <c r="F69" s="9" t="s">
-        <v>232</v>
+        <v>236</v>
       </c>
       <c r="G69" s="9" t="s">
-        <v>231</v>
+        <v>235</v>
       </c>
       <c r="H69" s="9" t="s">
         <v>13</v>
       </c>
       <c r="I69" s="9" t="s">
-        <v>233</v>
+        <v>237</v>
       </c>
     </row>
     <row r="70">
@@ -3390,28 +3414,28 @@
         <v>69.0</v>
       </c>
       <c r="B70" s="7" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="C70" s="8" t="s">
-        <v>235</v>
+        <v>239</v>
       </c>
       <c r="D70" s="9" t="s">
-        <v>236</v>
+        <v>240</v>
       </c>
       <c r="E70" s="9" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
       <c r="F70" s="9" t="s">
-        <v>238</v>
+        <v>242</v>
       </c>
       <c r="G70" s="9" t="s">
-        <v>236</v>
+        <v>240</v>
       </c>
       <c r="H70" s="9" t="s">
         <v>13</v>
       </c>
       <c r="I70" s="9" t="s">
-        <v>239</v>
+        <v>243</v>
       </c>
     </row>
     <row r="71">
@@ -3419,7 +3443,7 @@
         <v>70.0</v>
       </c>
       <c r="B71" s="7" t="s">
-        <v>240</v>
+        <v>244</v>
       </c>
       <c r="C71" s="10">
         <v>34.05</v>
@@ -3440,7 +3464,7 @@
         <v>13</v>
       </c>
       <c r="I71" s="9" t="s">
-        <v>241</v>
+        <v>245</v>
       </c>
     </row>
     <row r="72">
@@ -3448,28 +3472,28 @@
         <v>71.0</v>
       </c>
       <c r="B72" s="7" t="s">
-        <v>242</v>
+        <v>246</v>
       </c>
       <c r="C72" s="8" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="D72" s="9" t="s">
         <v>11</v>
       </c>
       <c r="E72" s="9" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="F72" s="9" t="s">
         <v>10</v>
       </c>
       <c r="G72" s="9" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="H72" s="9" t="s">
         <v>13</v>
       </c>
       <c r="I72" s="9" t="s">
-        <v>243</v>
+        <v>247</v>
       </c>
     </row>
     <row r="73">
@@ -3477,28 +3501,28 @@
         <v>72.0</v>
       </c>
       <c r="B73" s="7" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C73" s="8" t="s">
-        <v>244</v>
+        <v>248</v>
       </c>
       <c r="D73" s="9" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="E73" s="9" t="s">
-        <v>245</v>
+        <v>249</v>
       </c>
       <c r="F73" s="9" t="s">
         <v>17</v>
       </c>
       <c r="G73" s="9" t="s">
-        <v>245</v>
+        <v>249</v>
       </c>
       <c r="H73" s="9" t="s">
         <v>20</v>
       </c>
       <c r="I73" s="9" t="s">
-        <v>246</v>
+        <v>250</v>
       </c>
     </row>
     <row r="74">
@@ -3506,28 +3530,28 @@
         <v>73.0</v>
       </c>
       <c r="B74" s="7" t="s">
-        <v>247</v>
+        <v>251</v>
       </c>
       <c r="C74" s="8" t="s">
-        <v>248</v>
+        <v>252</v>
       </c>
       <c r="D74" s="9" t="s">
-        <v>249</v>
+        <v>253</v>
       </c>
       <c r="E74" s="9" t="s">
-        <v>250</v>
+        <v>254</v>
       </c>
       <c r="F74" s="9" t="s">
-        <v>251</v>
+        <v>255</v>
       </c>
       <c r="G74" s="9" t="s">
-        <v>249</v>
+        <v>253</v>
       </c>
       <c r="H74" s="9" t="s">
         <v>13</v>
       </c>
       <c r="I74" s="9" t="s">
-        <v>252</v>
+        <v>256</v>
       </c>
     </row>
     <row r="75">
@@ -3535,13 +3559,13 @@
         <v>74.0</v>
       </c>
       <c r="B75" s="7" t="s">
-        <v>253</v>
+        <v>257</v>
       </c>
       <c r="C75" s="8" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D75" s="9" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="E75" s="9" t="s">
         <v>32</v>
@@ -3556,7 +3580,7 @@
         <v>13</v>
       </c>
       <c r="I75" s="9" t="s">
-        <v>254</v>
+        <v>258</v>
       </c>
     </row>
     <row r="76">
@@ -3564,7 +3588,7 @@
         <v>75.0</v>
       </c>
       <c r="B76" s="7" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="C76" s="10">
         <v>1450.0</v>
@@ -3585,7 +3609,7 @@
         <v>13</v>
       </c>
       <c r="I76" s="9" t="s">
-        <v>255</v>
+        <v>259</v>
       </c>
     </row>
     <row r="77">
@@ -3593,7 +3617,7 @@
         <v>76.0</v>
       </c>
       <c r="B77" s="7" t="s">
-        <v>256</v>
+        <v>260</v>
       </c>
       <c r="C77" s="8" t="s">
         <v>10</v>
@@ -3614,7 +3638,7 @@
         <v>13</v>
       </c>
       <c r="I77" s="9" t="s">
-        <v>257</v>
+        <v>261</v>
       </c>
     </row>
     <row r="78">
@@ -3622,7 +3646,7 @@
         <v>77.0</v>
       </c>
       <c r="B78" s="7" t="s">
-        <v>258</v>
+        <v>262</v>
       </c>
       <c r="C78" s="8" t="s">
         <v>44</v>
@@ -3631,19 +3655,19 @@
         <v>19</v>
       </c>
       <c r="E78" s="9" t="s">
-        <v>259</v>
+        <v>263</v>
       </c>
       <c r="F78" s="9" t="s">
-        <v>260</v>
+        <v>264</v>
       </c>
       <c r="G78" s="9" t="s">
-        <v>260</v>
+        <v>264</v>
       </c>
       <c r="H78" s="9" t="s">
         <v>20</v>
       </c>
       <c r="I78" s="9" t="s">
-        <v>261</v>
+        <v>265</v>
       </c>
     </row>
     <row r="79">
@@ -3651,28 +3675,28 @@
         <v>78.0</v>
       </c>
       <c r="B79" s="7" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="C79" s="8" t="s">
-        <v>262</v>
+        <v>266</v>
       </c>
       <c r="D79" s="9" t="s">
-        <v>263</v>
+        <v>267</v>
       </c>
       <c r="E79" s="9" t="s">
-        <v>264</v>
+        <v>268</v>
       </c>
       <c r="F79" s="9" t="s">
-        <v>265</v>
+        <v>269</v>
       </c>
       <c r="G79" s="9" t="s">
-        <v>262</v>
+        <v>266</v>
       </c>
       <c r="H79" s="9" t="s">
         <v>13</v>
       </c>
       <c r="I79" s="9" t="s">
-        <v>266</v>
+        <v>270</v>
       </c>
     </row>
     <row r="80">
@@ -3680,10 +3704,10 @@
         <v>79.0</v>
       </c>
       <c r="B80" s="7" t="s">
-        <v>267</v>
+        <v>271</v>
       </c>
       <c r="C80" s="8" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D80" s="9" t="s">
         <v>31</v>
@@ -3692,7 +3716,7 @@
         <v>29</v>
       </c>
       <c r="F80" s="9" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="G80" s="9" t="s">
         <v>31</v>
@@ -3701,7 +3725,7 @@
         <v>13</v>
       </c>
       <c r="I80" s="9" t="s">
-        <v>268</v>
+        <v>272</v>
       </c>
     </row>
     <row r="81">
@@ -3709,7 +3733,7 @@
         <v>80.0</v>
       </c>
       <c r="B81" s="7" t="s">
-        <v>165</v>
+        <v>208</v>
       </c>
       <c r="C81" s="10">
         <v>31.59</v>
@@ -3730,7 +3754,7 @@
         <v>13</v>
       </c>
       <c r="I81" s="9" t="s">
-        <v>269</v>
+        <v>273</v>
       </c>
     </row>
     <row r="82">
@@ -3738,28 +3762,28 @@
         <v>81.0</v>
       </c>
       <c r="B82" s="7" t="s">
-        <v>270</v>
+        <v>274</v>
       </c>
       <c r="C82" s="8" t="s">
-        <v>271</v>
+        <v>275</v>
       </c>
       <c r="D82" s="9" t="s">
-        <v>272</v>
+        <v>276</v>
       </c>
       <c r="E82" s="9" t="s">
-        <v>273</v>
+        <v>277</v>
       </c>
       <c r="F82" s="9" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="G82" s="9" t="s">
-        <v>273</v>
+        <v>277</v>
       </c>
       <c r="H82" s="9" t="s">
         <v>13</v>
       </c>
       <c r="I82" s="9" t="s">
-        <v>275</v>
+        <v>279</v>
       </c>
     </row>
     <row r="83">
@@ -3767,28 +3791,28 @@
         <v>82.0</v>
       </c>
       <c r="B83" s="7" t="s">
-        <v>270</v>
+        <v>274</v>
       </c>
       <c r="C83" s="8" t="s">
-        <v>271</v>
+        <v>275</v>
       </c>
       <c r="D83" s="9" t="s">
-        <v>272</v>
+        <v>276</v>
       </c>
       <c r="E83" s="9" t="s">
-        <v>273</v>
+        <v>277</v>
       </c>
       <c r="F83" s="9" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="G83" s="9" t="s">
-        <v>271</v>
+        <v>275</v>
       </c>
       <c r="H83" s="9" t="s">
         <v>13</v>
       </c>
       <c r="I83" s="9" t="s">
-        <v>276</v>
+        <v>280</v>
       </c>
     </row>
     <row r="84">
@@ -3796,28 +3820,28 @@
         <v>83.0</v>
       </c>
       <c r="B84" s="7" t="s">
-        <v>270</v>
+        <v>274</v>
       </c>
       <c r="C84" s="8" t="s">
-        <v>271</v>
+        <v>275</v>
       </c>
       <c r="D84" s="9" t="s">
-        <v>272</v>
+        <v>276</v>
       </c>
       <c r="E84" s="9" t="s">
-        <v>273</v>
+        <v>277</v>
       </c>
       <c r="F84" s="9" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="G84" s="9" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="H84" s="9" t="s">
         <v>13</v>
       </c>
       <c r="I84" s="9" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
     </row>
     <row r="85">
@@ -3825,36 +3849,36 @@
         <v>84.0</v>
       </c>
       <c r="B85" s="7" t="s">
-        <v>270</v>
+        <v>274</v>
       </c>
       <c r="C85" s="8" t="s">
-        <v>271</v>
+        <v>275</v>
       </c>
       <c r="D85" s="9" t="s">
-        <v>272</v>
+        <v>276</v>
       </c>
       <c r="E85" s="9" t="s">
-        <v>273</v>
+        <v>277</v>
       </c>
       <c r="F85" s="9" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="G85" s="9" t="s">
-        <v>272</v>
+        <v>276</v>
       </c>
       <c r="H85" s="9" t="s">
         <v>13</v>
       </c>
       <c r="I85" s="9" t="s">
-        <v>278</v>
+        <v>282</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" s="6">
         <v>85.0</v>
       </c>
-      <c r="B86" s="7" t="s">
-        <v>279</v>
+      <c r="B86" s="12" t="s">
+        <v>283</v>
       </c>
       <c r="C86" s="10">
         <v>12.0</v>
@@ -3875,15 +3899,15 @@
         <v>13</v>
       </c>
       <c r="I86" s="9" t="s">
-        <v>280</v>
+        <v>284</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" s="6">
         <v>86.0</v>
       </c>
-      <c r="B87" s="7" t="s">
-        <v>279</v>
+      <c r="B87" s="12" t="s">
+        <v>283</v>
       </c>
       <c r="C87" s="10">
         <v>32.0</v>
@@ -3904,7 +3928,7 @@
         <v>13</v>
       </c>
       <c r="I87" s="9" t="s">
-        <v>281</v>
+        <v>285</v>
       </c>
     </row>
     <row r="88">
@@ -3912,7 +3936,7 @@
         <v>87.0</v>
       </c>
       <c r="B88" s="7" t="s">
-        <v>282</v>
+        <v>286</v>
       </c>
       <c r="C88" s="8" t="s">
         <v>29</v>
@@ -3924,16 +3948,16 @@
         <v>32</v>
       </c>
       <c r="F88" s="9" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="G88" s="9" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="H88" s="9" t="s">
         <v>20</v>
       </c>
       <c r="I88" s="9" t="s">
-        <v>283</v>
+        <v>287</v>
       </c>
     </row>
     <row r="89">
@@ -3941,13 +3965,13 @@
         <v>88.0</v>
       </c>
       <c r="B89" s="7" t="s">
-        <v>284</v>
+        <v>288</v>
       </c>
       <c r="C89" s="8" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="D89" s="9" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="E89" s="9" t="s">
         <v>32</v>
@@ -3956,13 +3980,13 @@
         <v>30</v>
       </c>
       <c r="G89" s="9" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="H89" s="9" t="s">
         <v>20</v>
       </c>
       <c r="I89" s="9" t="s">
-        <v>285</v>
+        <v>289</v>
       </c>
     </row>
     <row r="90">
@@ -3970,28 +3994,28 @@
         <v>89.0</v>
       </c>
       <c r="B90" s="7" t="s">
-        <v>284</v>
+        <v>288</v>
       </c>
       <c r="C90" s="8" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D90" s="9" t="s">
         <v>30</v>
       </c>
       <c r="E90" s="9" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="F90" s="9" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="G90" s="9" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="H90" s="9" t="s">
         <v>20</v>
       </c>
       <c r="I90" s="9" t="s">
-        <v>286</v>
+        <v>290</v>
       </c>
     </row>
     <row r="91">
@@ -3999,28 +4023,28 @@
         <v>90.0</v>
       </c>
       <c r="B91" s="7" t="s">
-        <v>284</v>
+        <v>288</v>
       </c>
       <c r="C91" s="8" t="s">
-        <v>287</v>
+        <v>291</v>
       </c>
       <c r="D91" s="9" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="E91" s="9" t="s">
         <v>32</v>
       </c>
       <c r="F91" s="9" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="G91" s="9" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="H91" s="9" t="s">
         <v>20</v>
       </c>
       <c r="I91" s="9" t="s">
-        <v>288</v>
+        <v>292</v>
       </c>
     </row>
     <row r="92">
@@ -4028,7 +4052,7 @@
         <v>91.0</v>
       </c>
       <c r="B92" s="7" t="s">
-        <v>279</v>
+        <v>293</v>
       </c>
       <c r="C92" s="10">
         <v>32.0</v>
@@ -4049,7 +4073,7 @@
         <v>20</v>
       </c>
       <c r="I92" s="9" t="s">
-        <v>289</v>
+        <v>294</v>
       </c>
     </row>
     <row r="93">
@@ -4057,28 +4081,28 @@
         <v>92.0</v>
       </c>
       <c r="B93" s="7" t="s">
-        <v>290</v>
+        <v>295</v>
       </c>
       <c r="C93" s="8" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="D93" s="9" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="E93" s="9" t="s">
         <v>32</v>
       </c>
       <c r="F93" s="9" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="G93" s="9" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="H93" s="9" t="s">
         <v>20</v>
       </c>
       <c r="I93" s="9" t="s">
-        <v>291</v>
+        <v>296</v>
       </c>
     </row>
     <row r="94">
@@ -4086,16 +4110,16 @@
         <v>93.0</v>
       </c>
       <c r="B94" s="7" t="s">
-        <v>290</v>
+        <v>295</v>
       </c>
       <c r="C94" s="8" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="D94" s="9" t="s">
         <v>31</v>
       </c>
       <c r="E94" s="9" t="s">
-        <v>292</v>
+        <v>297</v>
       </c>
       <c r="F94" s="9" t="s">
         <v>30</v>
@@ -4107,7 +4131,7 @@
         <v>20</v>
       </c>
       <c r="I94" s="9" t="s">
-        <v>293</v>
+        <v>298</v>
       </c>
     </row>
     <row r="95">
@@ -4115,19 +4139,19 @@
         <v>94.0</v>
       </c>
       <c r="B95" s="7" t="s">
-        <v>294</v>
+        <v>299</v>
       </c>
       <c r="C95" s="8" t="s">
         <v>17</v>
       </c>
       <c r="D95" s="9" t="s">
-        <v>295</v>
+        <v>300</v>
       </c>
       <c r="E95" s="9" t="s">
-        <v>244</v>
+        <v>248</v>
       </c>
       <c r="F95" s="9" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="G95" s="9" t="s">
         <v>17</v>
@@ -4136,7 +4160,7 @@
         <v>13</v>
       </c>
       <c r="I95" s="9" t="s">
-        <v>296</v>
+        <v>301</v>
       </c>
     </row>
     <row r="96">
@@ -4144,28 +4168,28 @@
         <v>95.0</v>
       </c>
       <c r="B96" s="7" t="s">
-        <v>297</v>
+        <v>302</v>
       </c>
       <c r="C96" s="8" t="s">
-        <v>244</v>
+        <v>248</v>
       </c>
       <c r="D96" s="9" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="E96" s="9" t="s">
-        <v>295</v>
+        <v>300</v>
       </c>
       <c r="F96" s="9" t="s">
         <v>17</v>
       </c>
       <c r="G96" s="9" t="s">
-        <v>295</v>
+        <v>300</v>
       </c>
       <c r="H96" s="9" t="s">
         <v>13</v>
       </c>
       <c r="I96" s="9" t="s">
-        <v>298</v>
+        <v>303</v>
       </c>
     </row>
     <row r="97">
@@ -4173,28 +4197,28 @@
         <v>96.0</v>
       </c>
       <c r="B97" s="7" t="s">
-        <v>297</v>
+        <v>302</v>
       </c>
       <c r="C97" s="8" t="s">
         <v>17</v>
       </c>
       <c r="D97" s="9" t="s">
-        <v>295</v>
+        <v>300</v>
       </c>
       <c r="E97" s="9" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="F97" s="9" t="s">
-        <v>244</v>
+        <v>248</v>
       </c>
       <c r="G97" s="9" t="s">
-        <v>244</v>
+        <v>248</v>
       </c>
       <c r="H97" s="9" t="s">
         <v>13</v>
       </c>
       <c r="I97" s="9" t="s">
-        <v>299</v>
+        <v>304</v>
       </c>
     </row>
     <row r="98">
@@ -4202,28 +4226,28 @@
         <v>97.0</v>
       </c>
       <c r="B98" s="7" t="s">
-        <v>297</v>
+        <v>299</v>
       </c>
       <c r="C98" s="8" t="s">
-        <v>244</v>
+        <v>248</v>
       </c>
       <c r="D98" s="9" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="E98" s="9" t="s">
-        <v>295</v>
+        <v>300</v>
       </c>
       <c r="F98" s="9" t="s">
         <v>17</v>
       </c>
       <c r="G98" s="9" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="H98" s="9" t="s">
         <v>13</v>
       </c>
       <c r="I98" s="9" t="s">
-        <v>300</v>
+        <v>305</v>
       </c>
     </row>
     <row r="99">
@@ -4231,7 +4255,7 @@
         <v>98.0</v>
       </c>
       <c r="B99" s="7" t="s">
-        <v>301</v>
+        <v>306</v>
       </c>
       <c r="C99" s="8" t="s">
         <v>11</v>
@@ -4252,7 +4276,7 @@
         <v>20</v>
       </c>
       <c r="I99" s="9" t="s">
-        <v>302</v>
+        <v>307</v>
       </c>
     </row>
     <row r="100">
@@ -4260,7 +4284,7 @@
         <v>99.0</v>
       </c>
       <c r="B100" s="7" t="s">
-        <v>303</v>
+        <v>308</v>
       </c>
       <c r="C100" s="10">
         <v>1.0</v>
@@ -4281,7 +4305,7 @@
         <v>20</v>
       </c>
       <c r="I100" s="9" t="s">
-        <v>304</v>
+        <v>309</v>
       </c>
     </row>
     <row r="101">
@@ -4289,7 +4313,7 @@
         <v>100.0</v>
       </c>
       <c r="B101" s="7" t="s">
-        <v>305</v>
+        <v>310</v>
       </c>
       <c r="C101" s="10">
         <v>1.0</v>
@@ -4310,7 +4334,7 @@
         <v>20</v>
       </c>
       <c r="I101" s="9" t="s">
-        <v>306</v>
+        <v>311</v>
       </c>
     </row>
     <row r="102">
@@ -4318,7 +4342,7 @@
         <v>101.0</v>
       </c>
       <c r="B102" s="7" t="s">
-        <v>303</v>
+        <v>308</v>
       </c>
       <c r="C102" s="10">
         <v>1.0</v>
@@ -4339,7 +4363,7 @@
         <v>20</v>
       </c>
       <c r="I102" s="9" t="s">
-        <v>307</v>
+        <v>312</v>
       </c>
     </row>
     <row r="103">
@@ -4347,7 +4371,7 @@
         <v>102.0</v>
       </c>
       <c r="B103" s="7" t="s">
-        <v>305</v>
+        <v>310</v>
       </c>
       <c r="C103" s="10">
         <v>1.0</v>
@@ -4368,7 +4392,7 @@
         <v>20</v>
       </c>
       <c r="I103" s="9" t="s">
-        <v>308</v>
+        <v>313</v>
       </c>
     </row>
     <row r="104">
@@ -4376,28 +4400,28 @@
         <v>103.0</v>
       </c>
       <c r="B104" s="7" t="s">
-        <v>309</v>
+        <v>314</v>
       </c>
       <c r="C104" s="8" t="s">
-        <v>310</v>
+        <v>315</v>
       </c>
       <c r="D104" s="9" t="s">
-        <v>311</v>
+        <v>316</v>
       </c>
       <c r="E104" s="9" t="s">
-        <v>312</v>
+        <v>317</v>
       </c>
       <c r="F104" s="9" t="s">
-        <v>235</v>
+        <v>239</v>
       </c>
       <c r="G104" s="9" t="s">
-        <v>312</v>
+        <v>317</v>
       </c>
       <c r="H104" s="9" t="s">
         <v>20</v>
       </c>
       <c r="I104" s="9" t="s">
-        <v>313</v>
+        <v>318</v>
       </c>
     </row>
     <row r="105">
@@ -4405,28 +4429,28 @@
         <v>104.0</v>
       </c>
       <c r="B105" s="7" t="s">
-        <v>314</v>
+        <v>319</v>
       </c>
       <c r="C105" s="8" t="s">
-        <v>315</v>
+        <v>320</v>
       </c>
       <c r="D105" s="9" t="s">
-        <v>316</v>
+        <v>321</v>
       </c>
       <c r="E105" s="9" t="s">
-        <v>317</v>
+        <v>322</v>
       </c>
       <c r="F105" s="9" t="s">
-        <v>318</v>
+        <v>323</v>
       </c>
       <c r="G105" s="9" t="s">
-        <v>319</v>
+        <v>324</v>
       </c>
       <c r="H105" s="9" t="s">
         <v>20</v>
       </c>
       <c r="I105" s="9" t="s">
-        <v>320</v>
+        <v>325</v>
       </c>
     </row>
     <row r="106">
@@ -4434,28 +4458,28 @@
         <v>105.0</v>
       </c>
       <c r="B106" s="7" t="s">
-        <v>314</v>
+        <v>319</v>
       </c>
       <c r="C106" s="8" t="s">
-        <v>318</v>
+        <v>323</v>
       </c>
       <c r="D106" s="9" t="s">
-        <v>317</v>
+        <v>322</v>
       </c>
       <c r="E106" s="9" t="s">
-        <v>315</v>
+        <v>320</v>
       </c>
       <c r="F106" s="9" t="s">
-        <v>316</v>
+        <v>321</v>
       </c>
       <c r="G106" s="9" t="s">
-        <v>315</v>
+        <v>320</v>
       </c>
       <c r="H106" s="9" t="s">
         <v>20</v>
       </c>
       <c r="I106" s="9" t="s">
-        <v>321</v>
+        <v>326</v>
       </c>
     </row>
     <row r="107">
@@ -4463,28 +4487,28 @@
         <v>106.0</v>
       </c>
       <c r="B107" s="7" t="s">
-        <v>314</v>
+        <v>319</v>
       </c>
       <c r="C107" s="8" t="s">
-        <v>235</v>
+        <v>239</v>
       </c>
       <c r="D107" s="9" t="s">
-        <v>312</v>
+        <v>317</v>
       </c>
       <c r="E107" s="9" t="s">
-        <v>322</v>
+        <v>327</v>
       </c>
       <c r="F107" s="9" t="s">
-        <v>323</v>
+        <v>328</v>
       </c>
       <c r="G107" s="9" t="s">
-        <v>323</v>
+        <v>328</v>
       </c>
       <c r="H107" s="9" t="s">
         <v>20</v>
       </c>
       <c r="I107" s="9" t="s">
-        <v>324</v>
+        <v>329</v>
       </c>
     </row>
     <row r="108">
@@ -4492,28 +4516,28 @@
         <v>107.0</v>
       </c>
       <c r="B108" s="7" t="s">
-        <v>325</v>
+        <v>330</v>
       </c>
       <c r="C108" s="8" t="s">
-        <v>326</v>
+        <v>331</v>
       </c>
       <c r="D108" s="9" t="s">
-        <v>327</v>
+        <v>332</v>
       </c>
       <c r="E108" s="9" t="s">
-        <v>328</v>
+        <v>333</v>
       </c>
       <c r="F108" s="9" t="s">
-        <v>329</v>
+        <v>334</v>
       </c>
       <c r="G108" s="9" t="s">
-        <v>326</v>
+        <v>331</v>
       </c>
       <c r="H108" s="9" t="s">
         <v>20</v>
       </c>
       <c r="I108" s="9" t="s">
-        <v>330</v>
+        <v>335</v>
       </c>
     </row>
     <row r="109">
@@ -4521,28 +4545,28 @@
         <v>108.0</v>
       </c>
       <c r="B109" s="7" t="s">
-        <v>325</v>
+        <v>330</v>
       </c>
       <c r="C109" s="8" t="s">
-        <v>327</v>
+        <v>332</v>
       </c>
       <c r="D109" s="9" t="s">
-        <v>328</v>
+        <v>333</v>
       </c>
       <c r="E109" s="9" t="s">
-        <v>326</v>
+        <v>331</v>
       </c>
       <c r="F109" s="9" t="s">
-        <v>329</v>
+        <v>334</v>
       </c>
       <c r="G109" s="9" t="s">
-        <v>328</v>
+        <v>333</v>
       </c>
       <c r="H109" s="9" t="s">
         <v>20</v>
       </c>
       <c r="I109" s="9" t="s">
-        <v>331</v>
+        <v>336</v>
       </c>
     </row>
     <row r="110">
@@ -4550,28 +4574,28 @@
         <v>109.0</v>
       </c>
       <c r="B110" s="7" t="s">
-        <v>325</v>
+        <v>330</v>
       </c>
       <c r="C110" s="8" t="s">
-        <v>328</v>
+        <v>333</v>
       </c>
       <c r="D110" s="9" t="s">
-        <v>326</v>
+        <v>331</v>
       </c>
       <c r="E110" s="9" t="s">
-        <v>327</v>
+        <v>332</v>
       </c>
       <c r="F110" s="9" t="s">
-        <v>329</v>
+        <v>334</v>
       </c>
       <c r="G110" s="9" t="s">
-        <v>327</v>
+        <v>332</v>
       </c>
       <c r="H110" s="9" t="s">
         <v>20</v>
       </c>
       <c r="I110" s="9" t="s">
-        <v>332</v>
+        <v>337</v>
       </c>
     </row>
     <row r="111">
@@ -4579,7 +4603,7 @@
         <v>110.0</v>
       </c>
       <c r="B111" s="7" t="s">
-        <v>333</v>
+        <v>338</v>
       </c>
       <c r="C111" s="10">
         <v>2.0</v>
@@ -4600,7 +4624,7 @@
         <v>20</v>
       </c>
       <c r="I111" s="9" t="s">
-        <v>334</v>
+        <v>339</v>
       </c>
     </row>
     <row r="112">
@@ -4608,7 +4632,7 @@
         <v>111.0</v>
       </c>
       <c r="B112" s="7" t="s">
-        <v>333</v>
+        <v>338</v>
       </c>
       <c r="C112" s="10">
         <v>1.0</v>
@@ -4629,7 +4653,7 @@
         <v>20</v>
       </c>
       <c r="I112" s="9" t="s">
-        <v>335</v>
+        <v>340</v>
       </c>
     </row>
     <row r="113">
@@ -4637,7 +4661,7 @@
         <v>112.0</v>
       </c>
       <c r="B113" s="7" t="s">
-        <v>333</v>
+        <v>338</v>
       </c>
       <c r="C113" s="10">
         <v>2.0</v>
@@ -4658,7 +4682,7 @@
         <v>20</v>
       </c>
       <c r="I113" s="9" t="s">
-        <v>336</v>
+        <v>341</v>
       </c>
     </row>
     <row r="114">
@@ -4666,7 +4690,7 @@
         <v>113.0</v>
       </c>
       <c r="B114" s="7" t="s">
-        <v>333</v>
+        <v>338</v>
       </c>
       <c r="C114" s="10">
         <v>1.0</v>
@@ -4687,7 +4711,7 @@
         <v>20</v>
       </c>
       <c r="I114" s="9" t="s">
-        <v>337</v>
+        <v>342</v>
       </c>
     </row>
     <row r="115">
@@ -4695,7 +4719,7 @@
         <v>114.0</v>
       </c>
       <c r="B115" s="7" t="s">
-        <v>333</v>
+        <v>338</v>
       </c>
       <c r="C115" s="10">
         <v>4.0</v>
@@ -4716,7 +4740,7 @@
         <v>20</v>
       </c>
       <c r="I115" s="9" t="s">
-        <v>338</v>
+        <v>343</v>
       </c>
     </row>
     <row r="116">
@@ -4724,7 +4748,7 @@
         <v>115.0</v>
       </c>
       <c r="B116" s="7" t="s">
-        <v>333</v>
+        <v>338</v>
       </c>
       <c r="C116" s="10">
         <v>2.0</v>
@@ -4745,7 +4769,7 @@
         <v>20</v>
       </c>
       <c r="I116" s="9" t="s">
-        <v>339</v>
+        <v>344</v>
       </c>
     </row>
     <row r="117">
@@ -4753,7 +4777,7 @@
         <v>116.0</v>
       </c>
       <c r="B117" s="7" t="s">
-        <v>333</v>
+        <v>338</v>
       </c>
       <c r="C117" s="10">
         <v>4.0</v>
@@ -4774,7 +4798,7 @@
         <v>20</v>
       </c>
       <c r="I117" s="9" t="s">
-        <v>340</v>
+        <v>345</v>
       </c>
     </row>
     <row r="118">
@@ -4782,7 +4806,7 @@
         <v>117.0</v>
       </c>
       <c r="B118" s="7" t="s">
-        <v>333</v>
+        <v>338</v>
       </c>
       <c r="C118" s="10">
         <v>3.0</v>
@@ -4803,7 +4827,7 @@
         <v>20</v>
       </c>
       <c r="I118" s="9" t="s">
-        <v>341</v>
+        <v>346</v>
       </c>
     </row>
     <row r="119">
@@ -4811,7 +4835,7 @@
         <v>118.0</v>
       </c>
       <c r="B119" s="7" t="s">
-        <v>333</v>
+        <v>338</v>
       </c>
       <c r="C119" s="10">
         <v>4.0</v>
@@ -4832,7 +4856,7 @@
         <v>20</v>
       </c>
       <c r="I119" s="9" t="s">
-        <v>342</v>
+        <v>347</v>
       </c>
     </row>
     <row r="120">
@@ -4840,7 +4864,7 @@
         <v>119.0</v>
       </c>
       <c r="B120" s="7" t="s">
-        <v>333</v>
+        <v>338</v>
       </c>
       <c r="C120" s="10">
         <v>1.0</v>
@@ -4861,7 +4885,7 @@
         <v>20</v>
       </c>
       <c r="I120" s="9" t="s">
-        <v>343</v>
+        <v>348</v>
       </c>
     </row>
     <row r="121">
@@ -4869,7 +4893,7 @@
         <v>120.0</v>
       </c>
       <c r="B121" s="7" t="s">
-        <v>333</v>
+        <v>338</v>
       </c>
       <c r="C121" s="10">
         <v>2.0</v>
@@ -4890,7 +4914,7 @@
         <v>20</v>
       </c>
       <c r="I121" s="9" t="s">
-        <v>344</v>
+        <v>349</v>
       </c>
     </row>
   </sheetData>

</xml_diff>